<commit_message>
Add documentation in the excel template
</commit_message>
<xml_diff>
--- a/src/tools/excel2yaml/template.xlsx
+++ b/src/tools/excel2yaml/template.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levi260/github/tools/src/tools/excel2yaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F3A512-844D-6445-B73D-1A94577C8A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1C57CF-5904-A047-A89E-60F58A99CA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{7E905681-4039-4FF9-85DA-8F8BE6699EA4}"/>
+    <workbookView xWindow="-36040" yWindow="-2640" windowWidth="34280" windowHeight="26240" xr2:uid="{7E905681-4039-4FF9-85DA-8F8BE6699EA4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="4" r:id="rId1"/>
-    <sheet name="Independent Variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Dependent Variables" sheetId="3" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="5" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="4" r:id="rId2"/>
+    <sheet name="Independent Variables" sheetId="2" r:id="rId3"/>
+    <sheet name="Dependent Variables" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
   <si>
     <t>Dataset Metadata</t>
   </si>
@@ -282,13 +283,617 @@
   </si>
   <si>
     <t>Doppler Spectral Broadening</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The goal of this tool is to simplify the process of creating dataset configuration files for tsdat ingests. There are two parts to this tool: 1) This Excel template file, which contains the metadata in a more user-friendly format, and 2) a command-line script that converts this Excel file into a YAML file format that can be read by tsdat.
+This Excel file contains 3 other sheets labeled "Metadata", "Independent Variables", and "Dependent Variables". Each sheet contains a table listing information for different parts of what wil be in the finalized dataset.
+- The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Metadata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet includes the global attributes for the dataset, typically describing the "what-when-where-how" of the collected input data. Information in this sheet exists in key-item pairs. Additional key-item pairs can be appended to new rows in this sheet.
+- The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Independent Variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet lists the variables that will become the "dimensions" or "coordinates" of the dataset – like time, depth, latitude, or longitude.
+- The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dependent Variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet lists the variables that are contained in the input data file.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Independent Variable Sheet Details</t>
+  </si>
+  <si>
+    <t>TZ database</t>
+  </si>
+  <si>
+    <t>CF conventions standard names</t>
+  </si>
+  <si>
+    <t>Dependent Variable Sheet Details</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>New Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The new (standardized) variable name. We recommend using underscores instead of spaces and keeping the name short.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Original Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The name of the variable in the raw input data file.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Standardized Unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The new variable unit.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Original Unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The variable unit in the input data file.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Timezone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Timezone identifier for "time" variables. Leave blank for other variables. See the TZ database for options.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Datatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Variable datatype (e.g., "float32").
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Long Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "Human-readable" version of the New Name.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Standard Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Name of the variable in the CF conventions lookup table, if there is a good match.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Additional metadata can be added as new columns on the right side of the sheet.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>New Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The new (standardized) variable name. We recommend using underscores instead of spaces and keeping the name short.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Original Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The name of the variable in the raw input data file.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Standardized Unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The new variable unit.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Original Unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The variable unit in the input data file.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Datatype</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Variable datatype (e.g., "float32").
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Dimensions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Independent variable(s) corresponding to the variable. Use commas to separate if multiple.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Long Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "Human-readable" version of the New Name.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Standard Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Name of the variable in the CF conventions lookup table, if there is a good match.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Valid Minimum Value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">: Lower range limit allowed for a variable, for quality control.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Valid Maximum Value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">: Upper range limit allowed for a variable, for quality control.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Additional metadata can be added as new columns on the right side of the sheet.</t>
+    </r>
+  </si>
+  <si>
+    <t>Template Overview</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Fill out the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Metadata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Independent Variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dependent Variable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">sheets in this Excel document and save the file.
+2) Install the "tsdat-tools" python package if you haven't already done so (requires python &gt;= 3.10):
+     &gt; pip install tsdat-tools
+3) Run the command-line utility to generate tsdat config files from this spreadsheet:
+     &gt; tsdat-tools excel2yaml run /path/to/this/template.xlsx
+If all goes well, this will generate two files: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>config/dataset.yaml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>config/retriever.yaml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. These are the primary configuration files needed by tsdat.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +925,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +993,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,10 +1047,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -418,8 +1081,41 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,10 +1427,785 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874C9F4C-5633-EB48-AC15-6A9E3F258451}">
+  <dimension ref="B1:T51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1" customWidth="1"/>
+    <col min="11" max="11" width="1.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="L1" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+    </row>
+    <row r="2" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+    </row>
+    <row r="3" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="L3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+    </row>
+    <row r="19" spans="2:20" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+    </row>
+    <row r="21" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="2:10" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="23"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+    </row>
+    <row r="38" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B38:J51"/>
+    <mergeCell ref="B22:J33"/>
+    <mergeCell ref="L1:T2"/>
+    <mergeCell ref="L3:T18"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="B36:J37"/>
+    <mergeCell ref="B1:J2"/>
+    <mergeCell ref="B20:J21"/>
+    <mergeCell ref="B3:J18"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" xr:uid="{C70E084D-1A09-A140-990A-AEE8E4009576}"/>
+    <hyperlink ref="C34" r:id="rId2" xr:uid="{84FD4A9E-254E-6D49-8EAF-88CDBA60DDC5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF81FB2-44A0-1B46-88A6-5034DCD6301E}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -761,7 +2232,7 @@
       <c r="A3" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C3" t="s">
@@ -770,7 +2241,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
-      <c r="B4" t="s">
+      <c r="B4" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -779,7 +2250,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
-      <c r="B5" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -788,7 +2259,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
-      <c r="B6" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -797,7 +2268,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
-      <c r="B7" t="s">
+      <c r="B7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -808,7 +2279,7 @@
       <c r="A8" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -817,7 +2288,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
-      <c r="B9" t="s">
+      <c r="B9" s="18" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -936,7 +2407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0564412-F11A-451E-9BE1-4FBFA691F3A7}">
   <dimension ref="A1:R4"/>
   <sheetViews>
@@ -1051,7 +2522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FD5847-269E-4516-8367-AFCCCB2514D0}">
   <dimension ref="A1:S9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Put the template back on the instructions page
</commit_message>
<xml_diff>
--- a/src/tools/excel2yaml/template.xlsx
+++ b/src/tools/excel2yaml/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levi260/github/tools/src/tools/excel2yaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54607CA-C97C-D948-A487-5699CE1A27D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D54C7AA-8FC7-144E-B975-C228D8CB39CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-3220" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{7E905681-4039-4FF9-85DA-8F8BE6699EA4}"/>
+    <workbookView xWindow="-51200" yWindow="-3220" windowWidth="51200" windowHeight="28300" xr2:uid="{7E905681-4039-4FF9-85DA-8F8BE6699EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -1558,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874C9F4C-5633-EB48-AC15-6A9E3F258451}">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:J2"/>
     </sheetView>
   </sheetViews>
@@ -2801,7 +2801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FD5847-269E-4516-8367-AFCCCB2514D0}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Fix data type dropdown after example row
</commit_message>
<xml_diff>
--- a/src/tools/excel2yaml/template.xlsx
+++ b/src/tools/excel2yaml/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/levi260/github/tools/src/tools/excel2yaml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10402B05-6BC1-8940-B34D-D64862F3D8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8807543A-1EBF-E045-BEA2-7C8A0CADD187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-3220" windowWidth="51200" windowHeight="28300" xr2:uid="{7E905681-4039-4FF9-85DA-8F8BE6699EA4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{7E905681-4039-4FF9-85DA-8F8BE6699EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -1206,6 +1206,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1219,9 +1222,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1550,472 +1550,472 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="L1" s="28" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="L1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
     </row>
     <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="L3" s="27" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="L3" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="27"/>
-      <c r="T17" s="27"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="27"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="27"/>
-      <c r="T19" s="27"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
     </row>
     <row r="23" spans="1:20" ht="7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="14"/>
@@ -2029,162 +2029,162 @@
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="19" t="s">
@@ -2210,217 +2210,217 @@
       <c r="J39" s="17"/>
     </row>
     <row r="40" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
     </row>
     <row r="41" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="29"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
     </row>
     <row r="42" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="28"/>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B55" s="27"/>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="27"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="27"/>
-      <c r="J56" s="27"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
-      <c r="J57" s="27"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="27"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2667,7 +2667,7 @@
       <c r="A1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="27" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2695,8 +2695,8 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:18" s="32" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:18" ht="34" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
@@ -2778,7 +2778,7 @@
           <x14:formula1>
             <xm:f>dtypes!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E6 E8 F9:F1048576 D3</xm:sqref>
+          <xm:sqref>E6 E8 E9:E1048576 D3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>